<commit_message>
v2.2 - bug fixes
- Fixed display power circuit with PNP (active low)
- Replace charger with MCP73781 (can toggle between 500mA and 1000mA with jumper)
- Fixed battery JST with PH connector
- Fixed 5V switch to switch before 5V boost instead of after to avoid voltage drop
- Merged 5V power with LED power
- Connected USB shield to ground
- Connected rotary encoder shield to ground
- Removed blue LED from 5V power to avoid voltage drop
- Thickened some power traces where needed
- Minor adjustments to traces, component placement and silkscreen to accommodate design changes
- Thickened mounting holes
- Added visible ground silkscreen for servo
- Renamed LEDs to match dotstar in code
- Better info in schematics where needed
- Updated dimensions, schematics, gerber, renders, BOM, 3D step files
- ERC/DRC done
</commit_message>
<xml_diff>
--- a/hardware/control_board/BORC_v2_control_board__BOM.xlsx
+++ b/hardware/control_board/BORC_v2_control_board__BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKstudios\Documents\GitHub\berg-lab BORC\hardware\control_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16DDF58-7B5B-46F5-9C2A-7D10D5950404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D4B80C-589E-4547-9EB7-45DBEF77D613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19185" yWindow="0" windowWidth="19200" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BORC_v2_control_board" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="202">
   <si>
     <t>Parts</t>
   </si>
@@ -136,9 +136,6 @@
     <t>915MHz</t>
   </si>
   <si>
-    <t>LED4, LED7, LED8, LED9, LED10, LED11</t>
-  </si>
-  <si>
     <t>U7</t>
   </si>
   <si>
@@ -148,15 +145,6 @@
     <t>ATMEGA1284P-MU</t>
   </si>
   <si>
-    <t>LED5</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>IN-S42ATB</t>
-  </si>
-  <si>
     <t>Q3, Q9, Q10</t>
   </si>
   <si>
@@ -169,9 +157,6 @@
     <t>FT231XQ-R</t>
   </si>
   <si>
-    <t>LED12</t>
-  </si>
-  <si>
     <t>GREEN</t>
   </si>
   <si>
@@ -214,9 +199,6 @@
     <t>J2</t>
   </si>
   <si>
-    <t>LED1, LED13</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
@@ -247,18 +229,12 @@
     <t>SSM3J374R,LF</t>
   </si>
   <si>
-    <t>Q1, Q4, Q16</t>
-  </si>
-  <si>
     <t>UMT3904T106</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>LED14</t>
-  </si>
-  <si>
     <t>YELLOW</t>
   </si>
   <si>
@@ -418,9 +394,6 @@
     <t>Inolux</t>
   </si>
   <si>
-    <t>Blue 470nm LED Indication - Discrete 3.1V 0402 (1005 Metric)</t>
-  </si>
-  <si>
     <t>N-Channel 60 V 320mA (Ta) 260mW (Ta), 830mW (Tc) Surface Mount SOT-323</t>
   </si>
   <si>
@@ -493,15 +466,6 @@
     <t>Red 631nm LED Indication - Discrete 2.1V 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>S2B-XH-A</t>
-  </si>
-  <si>
-    <t>Connector Header Through Hole, Right Angle 2 position 0.098" (2.50mm)</t>
-  </si>
-  <si>
-    <t>2 POS 2.5mm</t>
-  </si>
-  <si>
     <t>SHT40-BD1B-R3</t>
   </si>
   <si>
@@ -562,27 +526,12 @@
     <t>Yellow 592nm LED Indication - Discrete 1.9V 0402 (1005 Metric)</t>
   </si>
   <si>
-    <t>C2, C3, C4, C6, C9, C10, C11, C12, C13, C18, C21, C25, C26</t>
-  </si>
-  <si>
-    <t>R2, R8, R15, R16, R19, R20, R21, R22, R23, R24, R25, R28, R29, R30, R31, R32, R33, R35, R44, R45, R46, R47, R49, R50</t>
-  </si>
-  <si>
     <t>R3, R5, R17, R18</t>
   </si>
   <si>
-    <t>R1, R6, R7, R27, R36, R40, R48</t>
-  </si>
-  <si>
-    <t>Q1, Q2, Q5, Q7, Q11</t>
-  </si>
-  <si>
     <t>C15</t>
   </si>
   <si>
-    <t>C8, C20, C22, C24, C30, C32, C33</t>
-  </si>
-  <si>
     <t>MBR260HW</t>
   </si>
   <si>
@@ -598,15 +547,6 @@
     <t>Diode 60 V 2A Surface Mount SOD-123</t>
   </si>
   <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>MCP73833T-AMI/MF</t>
-  </si>
-  <si>
-    <t>Charger IC Lithium Ion/Polymer 10-DFN (3x3)</t>
-  </si>
-  <si>
     <t>Pololu Corporation</t>
   </si>
   <si>
@@ -614,6 +554,78 @@
   </si>
   <si>
     <t>U3V40F5</t>
+  </si>
+  <si>
+    <t>C2, C3, C4, C5, C6, C9, C10, C11, C12, C13, C18, C21, C25</t>
+  </si>
+  <si>
+    <t>LED0, LED1, LED2, LED3, LED4, LED5</t>
+  </si>
+  <si>
+    <t>LED8</t>
+  </si>
+  <si>
+    <t>LED6, LED7</t>
+  </si>
+  <si>
+    <t>LED9</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>RC0402FR-072KL</t>
+  </si>
+  <si>
+    <t>2 kOhms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>R34, R36</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OT</t>
+  </si>
+  <si>
+    <t>Charger IC Lithium Ion/Polymer SOT-23-5</t>
+  </si>
+  <si>
+    <t>S2B-PH-K-S</t>
+  </si>
+  <si>
+    <t>2 POS 2.0mm</t>
+  </si>
+  <si>
+    <t>Connector Header Through Hole, Right Angle 2 position 0.079" (2.00mm)</t>
+  </si>
+  <si>
+    <t>R2, R8, R15, R16, R19, R20, R21, R22, R23, R24, R25, R29, R35, R45, R46, R47, R49, R50</t>
+  </si>
+  <si>
+    <t>C8, C20, C22, C23, C24, C30</t>
+  </si>
+  <si>
+    <t>R1, R6, R7, R33, R48</t>
+  </si>
+  <si>
+    <t>Q5, Q11</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>BJT PNP 40V 0.2A</t>
+  </si>
+  <si>
+    <t>UMT3906T106</t>
+  </si>
+  <si>
+    <t>Bipolar (BJT) Transistor PNP 40 V 200 mA 250MHz 200 mW Surface Mount UMT3</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1145,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1150,16 +1162,13 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1221,9 +1230,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1261,7 +1270,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1367,7 +1376,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1509,7 +1518,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1517,7 +1526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1543,7 +1552,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -1552,7 +1561,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1563,10 +1572,10 @@
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1577,16 +1586,16 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1597,18 +1606,18 @@
         <v>10</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="8" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>180</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="B5" s="7">
         <v>13</v>
@@ -1617,16 +1626,16 @@
         <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1637,16 +1646,16 @@
         <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1657,16 +1666,16 @@
         <v>10</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1677,16 +1686,16 @@
         <v>100</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -1697,38 +1706,38 @@
         <v>18</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>181</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="24" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="B10" s="7">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B11" s="7">
         <v>4</v>
@@ -1737,18 +1746,18 @@
         <v>20</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -1757,36 +1766,36 @@
         <v>21</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B13" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -1797,478 +1806,478 @@
         <v>23</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
-        <v>183</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="B15" s="7">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>25</v>
+        <v>186</v>
       </c>
       <c r="B16" s="7">
         <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="D17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
         <v>220</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="D18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B18" s="7">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7">
-        <v>27</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="B19" s="7">
         <v>2</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>30</v>
+      <c r="C19" s="7">
+        <v>27</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="7">
         <v>2</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="7" t="s">
+      <c r="D21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" s="7">
+        <v>6</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="7" t="s">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="7">
-        <v>6</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="7">
-        <v>1</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="7">
-        <v>1</v>
-      </c>
-      <c r="C25" s="7" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="B27" s="7">
         <v>3</v>
       </c>
       <c r="C27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="F29" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="7">
-        <v>1</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F28" s="7" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="7">
-        <v>1</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="7">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="F34" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="7">
-        <v>1</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="7">
-        <v>1</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="7">
-        <v>1</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="B35" s="7">
-        <v>1</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="7">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="B37" s="7">
-        <v>1</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="B38" s="7">
         <v>1</v>
@@ -2277,213 +2286,233 @@
         <v>4012</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B39" s="7">
         <v>1</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>64</v>
+        <v>181</v>
       </c>
       <c r="B40" s="7">
         <v>2</v>
       </c>
       <c r="C40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="7">
-        <v>1</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="7">
-        <v>1</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="B43" s="7">
         <v>3</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="7">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B46" s="7">
+        <v>1</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="7">
+        <v>1</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="7">
+        <v>1</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="7">
+        <v>1</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B44" s="7">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B45" s="7">
-        <v>5</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="7">
-        <v>3</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="7">
-        <v>1</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="7">
-        <v>1</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>